<commit_message>
audio to separate class and some small changes
</commit_message>
<xml_diff>
--- a/Protocols/HeadingDiscrimination-avi.xlsx
+++ b/Protocols/HeadingDiscrimination-avi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\UniJoy\Protocols\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\Neuro-Lab-Project\Protocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -592,12 +592,24 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="62.25" customWidth="1"/>
+    <col min="10" max="10" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>